<commit_message>
First commit to add epoch time
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -17,105 +17,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="43">
-  <si>
-    <t>RID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="44">
+  <si>
+    <t>Readings ID</t>
+  </si>
+  <si>
+    <t>KWh Values</t>
+  </si>
+  <si>
+    <t>Power Factor</t>
+  </si>
+  <si>
+    <t>OrderDate</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Rep</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Pencil</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Kivell</t>
+  </si>
+  <si>
+    <t>Binder</t>
+  </si>
+  <si>
+    <t>Jardine</t>
+  </si>
+  <si>
+    <t>Gill</t>
+  </si>
+  <si>
+    <t>Pen</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Sorvino</t>
+  </si>
+  <si>
+    <t>Andrews</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Desk</t>
+  </si>
+  <si>
+    <t>Pen Set</t>
+  </si>
+  <si>
+    <t>Company ID</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Company Address</t>
+  </si>
+  <si>
+    <t>Company Assets</t>
   </si>
   <si>
     <t>KWh</t>
-  </si>
-  <si>
-    <t>Power Factor</t>
-  </si>
-  <si>
-    <t>OrderDate</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Rep</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Unit Cost</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>East</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>Pencil</t>
-  </si>
-  <si>
-    <t>Central</t>
-  </si>
-  <si>
-    <t>Kivell</t>
-  </si>
-  <si>
-    <t>Binder</t>
-  </si>
-  <si>
-    <t>Jardine</t>
-  </si>
-  <si>
-    <t>Gill</t>
-  </si>
-  <si>
-    <t>Pen</t>
-  </si>
-  <si>
-    <t>West</t>
-  </si>
-  <si>
-    <t>Sorvino</t>
-  </si>
-  <si>
-    <t>Andrews</t>
-  </si>
-  <si>
-    <t>Thompson</t>
-  </si>
-  <si>
-    <t>Morgan</t>
-  </si>
-  <si>
-    <t>Howard</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Desk</t>
-  </si>
-  <si>
-    <t>Pen Set</t>
-  </si>
-  <si>
-    <t>Company ID</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Company Address</t>
-  </si>
-  <si>
-    <t>Company Assets</t>
   </si>
   <si>
     <t>KVah</t>
@@ -156,9 +159,9 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="179" formatCode="hh:mm:ss;@"/>
     <numFmt numFmtId="180" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="181" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="181" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -199,16 +202,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Arial Narrow"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,26 +222,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -261,18 +260,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
       <i/>
@@ -292,51 +300,23 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial Narrow"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -349,11 +329,34 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -376,187 +379,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,17 +684,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -716,6 +708,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -734,23 +741,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -773,18 +765,29 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -797,135 +800,135 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -999,7 +1002,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1015,7 +1018,7 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1432,7 +1435,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -3073,10 +3076,10 @@
         <v>32</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3084,13 +3087,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>24.6</v>
@@ -3123,25 +3126,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3149,13 +3152,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" s="9">
         <v>26.8</v>

</xml_diff>